<commit_message>
improved coverage and fixed an unexpected behavior
</commit_message>
<xml_diff>
--- a/planning/gantt.xlsx
+++ b/planning/gantt.xlsx
@@ -1,48 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\Cours\BAC-3 -  Projet individuel\19-20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sloir/Documents/GitHub/2122_INFOB318_ESLintME/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAFCA06-5032-324D-9FE0-4694F7C4577B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15000" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="effort" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
-  <si>
-    <t>Analyse</t>
-  </si>
-  <si>
-    <t>Rencontre client</t>
-  </si>
-  <si>
-    <t>Correction</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Conception</t>
-  </si>
-  <si>
-    <t>correction</t>
-  </si>
-  <si>
-    <t>code round</t>
-  </si>
-  <si>
-    <t>test &amp; fix</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t>Total/Semaine</t>
@@ -66,22 +58,61 @@
     <t>Projet:</t>
   </si>
   <si>
-    <t>Rédaction de la documentation</t>
-  </si>
-  <si>
-    <t>Préparation de la présentation</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
     <t>Tampon récupération retard</t>
   </si>
+  <si>
+    <t>Loir</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>ESLintME</t>
+  </si>
+  <si>
+    <t>Recherche initiale sur ESLint</t>
+  </si>
+  <si>
+    <t>Analyse des besoins + choix des outils</t>
+  </si>
+  <si>
+    <t>Première réunion avec le client (14/10)</t>
+  </si>
+  <si>
+    <t>Deuxième réunion avec le client (28/10)</t>
+  </si>
+  <si>
+    <t>Troisième réunion avec le client (18/11)</t>
+  </si>
+  <si>
+    <t>Quatrième réunion avec le client (9/12)</t>
+  </si>
+  <si>
+    <t>Dernière réunion avec le client (21/02)</t>
+  </si>
+  <si>
+    <t>Finalisation des tests</t>
+  </si>
+  <si>
+    <t>Préparation des exécutables</t>
+  </si>
+  <si>
+    <t>Correction de bugs / problèmes UI/UX</t>
+  </si>
+  <si>
+    <t>Conception des dernières fonctionnalités</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,12 +600,12 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="5" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="8" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="5" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30"/>
@@ -673,6 +704,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -708,6 +756,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -883,101 +948,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AH46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:AH47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:34" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="2:34" ht="21" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="2:34" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="21" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="2:34" ht="21" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="2:34" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" spans="2:34" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="2:34" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" s="19">
-        <f>SUM(D11:D36)</f>
-        <v>13</v>
+        <f>SUM(D11:D37)</f>
+        <v>4</v>
       </c>
       <c r="E7" s="20">
-        <f t="shared" ref="E7:Z7" si="0">SUM(E11:E36)</f>
-        <v>12</v>
+        <f t="shared" ref="E7:Z7" si="0">SUM(E11:E37)</f>
+        <v>0</v>
       </c>
       <c r="F7" s="20">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" s="20">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="0"/>
@@ -989,7 +1062,7 @@
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
@@ -1033,14 +1106,14 @@
       </c>
       <c r="Y7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA7" s="6">
-        <f t="shared" ref="AA7:AH7" si="1">SUM(AA11:AA36)</f>
+        <f t="shared" ref="AA7:AH7" si="1">SUM(AA11:AA37)</f>
         <v>0</v>
       </c>
       <c r="AB7" s="6">
@@ -1072,287 +1145,283 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>43723</v>
+        <v>44466</v>
       </c>
       <c r="E8" s="2">
         <f>D8+7</f>
-        <v>43730</v>
+        <v>44473</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ref="F8:Q8" si="2">E8+7</f>
-        <v>43737</v>
+        <v>44480</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="2"/>
-        <v>43744</v>
+        <v>44487</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>43751</v>
+        <v>44494</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>43758</v>
+        <v>44501</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="2"/>
-        <v>43765</v>
+        <v>44508</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="2"/>
-        <v>43772</v>
+        <v>44515</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="2"/>
-        <v>43779</v>
+        <v>44522</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="2"/>
-        <v>43786</v>
+        <v>44529</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="2"/>
-        <v>43793</v>
+        <v>44536</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="2"/>
-        <v>43800</v>
+        <v>44543</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="2"/>
-        <v>43807</v>
+        <v>44550</v>
       </c>
       <c r="Q8" s="3">
         <f t="shared" si="2"/>
-        <v>43814</v>
+        <v>44557</v>
       </c>
       <c r="R8" s="3">
         <f t="shared" ref="R8" si="3">Q8+7</f>
-        <v>43821</v>
+        <v>44564</v>
       </c>
       <c r="S8" s="3">
         <f t="shared" ref="S8" si="4">R8+7</f>
-        <v>43828</v>
+        <v>44571</v>
       </c>
       <c r="T8" s="3">
         <f t="shared" ref="T8" si="5">S8+7</f>
-        <v>43835</v>
+        <v>44578</v>
       </c>
       <c r="U8" s="3">
         <f t="shared" ref="U8" si="6">T8+7</f>
-        <v>43842</v>
+        <v>44585</v>
       </c>
       <c r="V8" s="3">
         <f t="shared" ref="V8" si="7">U8+7</f>
-        <v>43849</v>
+        <v>44592</v>
       </c>
       <c r="W8" s="3">
         <f t="shared" ref="W8" si="8">V8+7</f>
-        <v>43856</v>
+        <v>44599</v>
       </c>
       <c r="X8" s="3">
         <f t="shared" ref="X8" si="9">W8+7</f>
-        <v>43863</v>
+        <v>44606</v>
       </c>
       <c r="Y8" s="3">
         <f t="shared" ref="Y8" si="10">X8+7</f>
-        <v>43870</v>
+        <v>44613</v>
       </c>
       <c r="Z8" s="3">
         <f t="shared" ref="Z8:AH8" si="11">Y8+7</f>
-        <v>43877</v>
+        <v>44620</v>
       </c>
       <c r="AA8" s="3">
         <f t="shared" si="11"/>
-        <v>43884</v>
+        <v>44627</v>
       </c>
       <c r="AB8" s="3">
         <f t="shared" si="11"/>
-        <v>43891</v>
+        <v>44634</v>
       </c>
       <c r="AC8" s="3">
         <f t="shared" si="11"/>
-        <v>43898</v>
+        <v>44641</v>
       </c>
       <c r="AD8" s="3">
         <f t="shared" si="11"/>
-        <v>43905</v>
+        <v>44648</v>
       </c>
       <c r="AE8" s="3">
         <f t="shared" si="11"/>
-        <v>43912</v>
+        <v>44655</v>
       </c>
       <c r="AF8" s="3">
         <f t="shared" si="11"/>
-        <v>43919</v>
+        <v>44662</v>
       </c>
       <c r="AG8" s="3">
         <f t="shared" si="11"/>
-        <v>43926</v>
+        <v>44669</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" si="11"/>
-        <v>43933</v>
-      </c>
-    </row>
-    <row r="9" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C9" s="22">
-        <f>SUM(C10:C46)</f>
-        <v>60</v>
-      </c>
-      <c r="D9" s="27">
-        <f>SUM(D10:D46)</f>
-        <v>14</v>
-      </c>
-      <c r="E9" s="27">
-        <f t="shared" ref="E9:Z9" si="12">SUM(E10:E46)</f>
+        <f>SUM(C10:C47)</f>
+        <v>42</v>
+      </c>
+      <c r="D9" s="26">
+        <f>SUM(D10:D47)</f>
+        <v>4</v>
+      </c>
+      <c r="E9" s="26">
+        <f t="shared" ref="E9:Z9" si="12">SUM(E10:E47)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="26">
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
-      <c r="F9" s="27">
+      <c r="G9" s="26">
         <f t="shared" si="12"/>
-        <v>11</v>
-      </c>
-      <c r="G9" s="27">
+        <v>2</v>
+      </c>
+      <c r="H9" s="26">
         <f t="shared" si="12"/>
-        <v>11</v>
-      </c>
-      <c r="H9" s="27">
+        <v>4</v>
+      </c>
+      <c r="I9" s="26">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="26">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="26">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I9" s="27">
+      <c r="L9" s="26">
         <f t="shared" si="12"/>
-        <v>7</v>
-      </c>
-      <c r="J9" s="27">
+        <v>0</v>
+      </c>
+      <c r="M9" s="26">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="K9" s="27">
+        <v>0</v>
+      </c>
+      <c r="N9" s="26">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="27">
+        <v>1</v>
+      </c>
+      <c r="O9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M9" s="27">
+      <c r="P9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="N9" s="27">
+      <c r="Q9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O9" s="27">
+      <c r="R9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P9" s="27">
+      <c r="S9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="27">
+      <c r="T9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="R9" s="27">
+      <c r="U9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="S9" s="27">
+      <c r="V9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="T9" s="27">
+      <c r="W9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="U9" s="27">
+      <c r="X9" s="26">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="V9" s="27">
+      <c r="Y9" s="26">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="W9" s="27">
+        <v>10</v>
+      </c>
+      <c r="Z9" s="26">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="X9" s="27">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="27">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="27">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="27">
-        <f t="shared" ref="AA9:AH9" si="13">SUM(AA10:AA46)</f>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="27">
+        <v>8</v>
+      </c>
+      <c r="AA9" s="26">
+        <f t="shared" ref="AA9:AH9" si="13">SUM(AA10:AA47)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AC9" s="27">
+      <c r="AC9" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD9" s="27">
+      <c r="AD9" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="27">
+      <c r="AE9" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AF9" s="27">
+      <c r="AF9" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="27">
+      <c r="AG9" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AH9" s="27">
+      <c r="AH9" s="26">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="26">
+    <row r="10" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="25">
         <f>SUM(D10:AH10)</f>
-        <v>2</v>
-      </c>
-      <c r="D10" s="16">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D10" s="16"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="10">
-        <v>1</v>
-      </c>
+      <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -1380,16 +1449,16 @@
       <c r="AG10" s="11"/>
       <c r="AH10" s="11"/>
     </row>
-    <row r="11" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="26">
-        <f t="shared" ref="C11:C46" si="14">SUM(D11:AH11)</f>
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="25">
+        <f t="shared" ref="C11:C47" si="14">SUM(D11:AH11)</f>
+        <v>4</v>
       </c>
       <c r="D11" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1422,21 +1491,19 @@
       <c r="AG11" s="13"/>
       <c r="AH11" s="13"/>
     </row>
-    <row r="12" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="26">
+        <v>16</v>
+      </c>
+      <c r="C12" s="25">
         <f t="shared" si="14"/>
-        <v>24</v>
-      </c>
-      <c r="D12" s="17">
-        <v>12</v>
-      </c>
-      <c r="E12" s="12">
-        <v>12</v>
-      </c>
-      <c r="F12" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12">
+        <v>1</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -1466,18 +1533,18 @@
       <c r="AG12" s="13"/>
       <c r="AH12" s="13"/>
     </row>
-    <row r="13" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="26">
+        <v>15</v>
+      </c>
+      <c r="C13" s="25">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -1508,21 +1575,25 @@
       <c r="AG13" s="13"/>
       <c r="AH13" s="13"/>
     </row>
-    <row r="14" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="26">
+        <v>0</v>
+      </c>
+      <c r="C14" s="25">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12">
+        <v>7</v>
+      </c>
+      <c r="G14" s="12">
+        <v>2</v>
+      </c>
+      <c r="H14" s="12">
         <v>3</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1550,21 +1621,21 @@
       <c r="AG14" s="13"/>
       <c r="AH14" s="13"/>
     </row>
-    <row r="15" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="26">
+        <v>17</v>
+      </c>
+      <c r="C15" s="25">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="12">
-        <v>7</v>
-      </c>
+      <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="12">
+        <v>1</v>
+      </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1592,20 +1663,18 @@
       <c r="AG15" s="13"/>
       <c r="AH15" s="13"/>
     </row>
-    <row r="16" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="26">
+        <v>0</v>
+      </c>
+      <c r="C16" s="25">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="12">
-        <v>1</v>
-      </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -1634,24 +1703,24 @@
       <c r="AG16" s="13"/>
       <c r="AH16" s="13"/>
     </row>
-    <row r="17" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="26">
+        <v>18</v>
+      </c>
+      <c r="C17" s="25">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="12">
-        <v>3</v>
-      </c>
+      <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="K17" s="12">
+        <v>1</v>
+      </c>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
@@ -1676,24 +1745,20 @@
       <c r="AG17" s="13"/>
       <c r="AH17" s="13"/>
     </row>
-    <row r="18" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="26">
+        <v>0</v>
+      </c>
+      <c r="C18" s="25">
         <f t="shared" si="14"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="12">
-        <v>7</v>
-      </c>
+      <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="12">
-        <v>7</v>
-      </c>
+      <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -1720,13 +1785,13 @@
       <c r="AG18" s="13"/>
       <c r="AH18" s="13"/>
     </row>
-    <row r="19" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="26">
+        <v>19</v>
+      </c>
+      <c r="C19" s="25">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="12"/>
@@ -1734,13 +1799,13 @@
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
-      <c r="J19" s="12">
-        <v>3</v>
-      </c>
+      <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="N19" s="12">
+        <v>1</v>
+      </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
@@ -1762,13 +1827,13 @@
       <c r="AG19" s="13"/>
       <c r="AH19" s="13"/>
     </row>
-    <row r="20" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="26">
+        <v>0</v>
+      </c>
+      <c r="C20" s="25">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="12"/>
@@ -1776,9 +1841,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
-      <c r="J20" s="12">
-        <v>1</v>
-      </c>
+      <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
@@ -1804,13 +1867,13 @@
       <c r="AG20" s="13"/>
       <c r="AH20" s="13"/>
     </row>
-    <row r="21" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="26">
+        <v>20</v>
+      </c>
+      <c r="C21" s="25">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="12"/>
@@ -1833,7 +1896,9 @@
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
+      <c r="Y21" s="12">
+        <v>1</v>
+      </c>
       <c r="Z21" s="13"/>
       <c r="AA21" s="13"/>
       <c r="AB21" s="13"/>
@@ -1844,13 +1909,13 @@
       <c r="AG21" s="13"/>
       <c r="AH21" s="13"/>
     </row>
-    <row r="22" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="26">
+        <v>24</v>
+      </c>
+      <c r="C22" s="25">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="12"/>
@@ -1873,7 +1938,9 @@
       <c r="V22" s="12"/>
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
+      <c r="Y22" s="12">
+        <v>3</v>
+      </c>
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
       <c r="AB22" s="13"/>
@@ -1884,13 +1951,13 @@
       <c r="AG22" s="13"/>
       <c r="AH22" s="13"/>
     </row>
-    <row r="23" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="26">
+        <v>23</v>
+      </c>
+      <c r="C23" s="25">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="12"/>
@@ -1913,7 +1980,9 @@
       <c r="V23" s="12"/>
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
+      <c r="Y23" s="12">
+        <v>6</v>
+      </c>
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
       <c r="AB23" s="13"/>
@@ -1924,13 +1993,13 @@
       <c r="AG23" s="13"/>
       <c r="AH23" s="13"/>
     </row>
-    <row r="24" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="26">
+        <v>21</v>
+      </c>
+      <c r="C24" s="25">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="12"/>
@@ -1954,7 +2023,9 @@
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
-      <c r="Z24" s="13"/>
+      <c r="Z24" s="13">
+        <v>5</v>
+      </c>
       <c r="AA24" s="13"/>
       <c r="AB24" s="13"/>
       <c r="AC24" s="13"/>
@@ -1964,13 +2035,13 @@
       <c r="AG24" s="13"/>
       <c r="AH24" s="13"/>
     </row>
-    <row r="25" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="26">
+        <v>22</v>
+      </c>
+      <c r="C25" s="25">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="12"/>
@@ -1994,7 +2065,9 @@
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
-      <c r="Z25" s="13"/>
+      <c r="Z25" s="13">
+        <v>3</v>
+      </c>
       <c r="AA25" s="13"/>
       <c r="AB25" s="13"/>
       <c r="AC25" s="13"/>
@@ -2004,11 +2077,9 @@
       <c r="AG25" s="13"/>
       <c r="AH25" s="13"/>
     </row>
-    <row r="26" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="26">
+    <row r="26" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2044,11 +2115,9 @@
       <c r="AG26" s="13"/>
       <c r="AH26" s="13"/>
     </row>
-    <row r="27" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="26">
+    <row r="27" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2084,11 +2153,9 @@
       <c r="AG27" s="13"/>
       <c r="AH27" s="13"/>
     </row>
-    <row r="28" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="26">
+    <row r="28" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2124,9 +2191,9 @@
       <c r="AG28" s="13"/>
       <c r="AH28" s="13"/>
     </row>
-    <row r="29" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
-      <c r="C29" s="26">
+      <c r="C29" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2162,9 +2229,9 @@
       <c r="AG29" s="13"/>
       <c r="AH29" s="13"/>
     </row>
-    <row r="30" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
-      <c r="C30" s="26">
+      <c r="C30" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2200,9 +2267,9 @@
       <c r="AG30" s="13"/>
       <c r="AH30" s="13"/>
     </row>
-    <row r="31" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="26">
+      <c r="C31" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2238,9 +2305,9 @@
       <c r="AG31" s="13"/>
       <c r="AH31" s="13"/>
     </row>
-    <row r="32" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
-      <c r="C32" s="26">
+      <c r="C32" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2276,9 +2343,9 @@
       <c r="AG32" s="13"/>
       <c r="AH32" s="13"/>
     </row>
-    <row r="33" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
-      <c r="C33" s="26">
+      <c r="C33" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2314,9 +2381,9 @@
       <c r="AG33" s="13"/>
       <c r="AH33" s="13"/>
     </row>
-    <row r="34" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
-      <c r="C34" s="26">
+      <c r="C34" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2352,9 +2419,9 @@
       <c r="AG34" s="13"/>
       <c r="AH34" s="13"/>
     </row>
-    <row r="35" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="8"/>
-      <c r="C35" s="26">
+    <row r="35" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2390,11 +2457,9 @@
       <c r="AG35" s="13"/>
       <c r="AH35" s="13"/>
     </row>
-    <row r="36" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="26">
+    <row r="36" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2430,11 +2495,9 @@
       <c r="AG36" s="13"/>
       <c r="AH36" s="13"/>
     </row>
-    <row r="37" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="26">
+    <row r="37" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+      <c r="C37" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2470,11 +2533,9 @@
       <c r="AG37" s="13"/>
       <c r="AH37" s="13"/>
     </row>
-    <row r="38" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="26">
+    <row r="38" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+      <c r="C38" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2510,11 +2571,9 @@
       <c r="AG38" s="13"/>
       <c r="AH38" s="13"/>
     </row>
-    <row r="39" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="26">
+    <row r="39" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+      <c r="C39" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2550,9 +2609,9 @@
       <c r="AG39" s="13"/>
       <c r="AH39" s="13"/>
     </row>
-    <row r="40" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
-      <c r="C40" s="26">
+      <c r="C40" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2588,9 +2647,9 @@
       <c r="AG40" s="13"/>
       <c r="AH40" s="13"/>
     </row>
-    <row r="41" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
-      <c r="C41" s="26">
+      <c r="C41" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2626,9 +2685,9 @@
       <c r="AG41" s="13"/>
       <c r="AH41" s="13"/>
     </row>
-    <row r="42" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
-      <c r="C42" s="26">
+      <c r="C42" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2664,9 +2723,9 @@
       <c r="AG42" s="13"/>
       <c r="AH42" s="13"/>
     </row>
-    <row r="43" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
-      <c r="C43" s="26">
+      <c r="C43" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2702,9 +2761,9 @@
       <c r="AG43" s="13"/>
       <c r="AH43" s="13"/>
     </row>
-    <row r="44" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
-      <c r="C44" s="26">
+      <c r="C44" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2740,9 +2799,9 @@
       <c r="AG44" s="13"/>
       <c r="AH44" s="13"/>
     </row>
-    <row r="45" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
-      <c r="C45" s="26">
+      <c r="C45" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -2778,43 +2837,81 @@
       <c r="AG45" s="13"/>
       <c r="AH45" s="13"/>
     </row>
-    <row r="46" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="8"/>
-      <c r="C46" s="26">
+    <row r="46" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
+      <c r="C46" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
-      <c r="T46" s="14"/>
-      <c r="U46" s="14"/>
-      <c r="V46" s="14"/>
-      <c r="W46" s="14"/>
-      <c r="X46" s="14"/>
-      <c r="Y46" s="14"/>
-      <c r="Z46" s="15"/>
-      <c r="AA46" s="15"/>
-      <c r="AB46" s="15"/>
-      <c r="AC46" s="15"/>
-      <c r="AD46" s="15"/>
-      <c r="AE46" s="15"/>
-      <c r="AF46" s="15"/>
-      <c r="AG46" s="15"/>
-      <c r="AH46" s="15"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="13"/>
+      <c r="AC46" s="13"/>
+      <c r="AD46" s="13"/>
+      <c r="AE46" s="13"/>
+      <c r="AF46" s="13"/>
+      <c r="AG46" s="13"/>
+      <c r="AH46" s="13"/>
+    </row>
+    <row r="47" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="8"/>
+      <c r="C47" s="25">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="18"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+      <c r="Z47" s="15"/>
+      <c r="AA47" s="15"/>
+      <c r="AB47" s="15"/>
+      <c r="AC47" s="15"/>
+      <c r="AD47" s="15"/>
+      <c r="AE47" s="15"/>
+      <c r="AF47" s="15"/>
+      <c r="AG47" s="15"/>
+      <c r="AH47" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2823,7 +2920,7 @@
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D11:P18 D21:P29 D19:H20 J19:P20">
+  <conditionalFormatting sqref="D11:P18 D21:P30 D19:H20 J19:P20">
     <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
@@ -2833,7 +2930,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:Q10 Q11:Q29">
+  <conditionalFormatting sqref="D10:Q10 Q11:Q30">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
@@ -2843,7 +2940,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R10:Z29">
+  <conditionalFormatting sqref="R10:Z30">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
@@ -2867,7 +2964,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:P30">
+  <conditionalFormatting sqref="D31:P31">
     <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
@@ -2877,7 +2974,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q30">
+  <conditionalFormatting sqref="Q31">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
@@ -2887,7 +2984,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R30:Z30">
+  <conditionalFormatting sqref="R31:Z31">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -2897,7 +2994,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:P35">
+  <conditionalFormatting sqref="D32:P36">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -2907,7 +3004,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q31:Q35">
+  <conditionalFormatting sqref="Q32:Q36">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -2917,7 +3014,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R31:Z35">
+  <conditionalFormatting sqref="R32:Z36">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -2927,7 +3024,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:P40">
+  <conditionalFormatting sqref="D37:P41">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -2937,7 +3034,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q36:Q40">
+  <conditionalFormatting sqref="Q37:Q41">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -2947,7 +3044,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R36:Z40">
+  <conditionalFormatting sqref="R37:Z41">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -2957,7 +3054,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:P41">
+  <conditionalFormatting sqref="D42:P42">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -2967,7 +3064,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q41">
+  <conditionalFormatting sqref="Q42">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -2977,7 +3074,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R41:Z41">
+  <conditionalFormatting sqref="R42:Z42">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -2987,7 +3084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42:P46">
+  <conditionalFormatting sqref="D43:P47">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -2997,7 +3094,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q42:Q46">
+  <conditionalFormatting sqref="Q43:Q47">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -3007,7 +3104,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R42:Z46">
+  <conditionalFormatting sqref="R43:Z47">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -3017,7 +3114,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA10:AA29">
+  <conditionalFormatting sqref="AA10:AA30">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -3027,7 +3124,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA30">
+  <conditionalFormatting sqref="AA31">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -3037,7 +3134,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA31:AA35">
+  <conditionalFormatting sqref="AA32:AA36">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -3047,7 +3144,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA36:AA40">
+  <conditionalFormatting sqref="AA37:AA41">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -3057,7 +3154,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA41">
+  <conditionalFormatting sqref="AA42">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -3067,7 +3164,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA42:AA46">
+  <conditionalFormatting sqref="AA43:AA47">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -3077,7 +3174,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB10:AB29">
+  <conditionalFormatting sqref="AB10:AB30">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -3087,7 +3184,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB30">
+  <conditionalFormatting sqref="AB31">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -3097,7 +3194,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB31:AB35">
+  <conditionalFormatting sqref="AB32:AB36">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -3107,7 +3204,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB36:AB40">
+  <conditionalFormatting sqref="AB37:AB41">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -3117,7 +3214,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB41">
+  <conditionalFormatting sqref="AB42">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -3127,7 +3224,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB42:AB46">
+  <conditionalFormatting sqref="AB43:AB47">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -3137,7 +3234,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC10:AC29">
+  <conditionalFormatting sqref="AC10:AC30">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -3147,7 +3244,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC30">
+  <conditionalFormatting sqref="AC31">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -3157,7 +3254,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC31:AC35">
+  <conditionalFormatting sqref="AC32:AC36">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -3167,7 +3264,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC36:AC40">
+  <conditionalFormatting sqref="AC37:AC41">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -3177,7 +3274,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC41">
+  <conditionalFormatting sqref="AC42">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -3187,7 +3284,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC42:AC46">
+  <conditionalFormatting sqref="AC43:AC47">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -3197,7 +3294,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD10:AD29">
+  <conditionalFormatting sqref="AD10:AD30">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -3207,7 +3304,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD30">
+  <conditionalFormatting sqref="AD31">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -3217,7 +3314,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD31:AD35">
+  <conditionalFormatting sqref="AD32:AD36">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -3227,7 +3324,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD36:AD40">
+  <conditionalFormatting sqref="AD37:AD41">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -3237,7 +3334,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD41">
+  <conditionalFormatting sqref="AD42">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -3247,7 +3344,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD42:AD46">
+  <conditionalFormatting sqref="AD43:AD47">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -3257,7 +3354,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE10:AE29">
+  <conditionalFormatting sqref="AE10:AE30">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -3267,7 +3364,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE30">
+  <conditionalFormatting sqref="AE31">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -3277,7 +3374,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE31:AE35">
+  <conditionalFormatting sqref="AE32:AE36">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -3287,7 +3384,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE36:AE40">
+  <conditionalFormatting sqref="AE37:AE41">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3297,7 +3394,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE41">
+  <conditionalFormatting sqref="AE42">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -3307,7 +3404,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE42:AE46">
+  <conditionalFormatting sqref="AE43:AE47">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3317,7 +3414,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF10:AF29">
+  <conditionalFormatting sqref="AF10:AF30">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3327,7 +3424,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF30">
+  <conditionalFormatting sqref="AF31">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -3337,7 +3434,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF31:AF35">
+  <conditionalFormatting sqref="AF32:AF36">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3347,7 +3444,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF36:AF40">
+  <conditionalFormatting sqref="AF37:AF41">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3357,7 +3454,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF41">
+  <conditionalFormatting sqref="AF42">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3367,7 +3464,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF42:AF46">
+  <conditionalFormatting sqref="AF43:AF47">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -3377,7 +3474,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG10:AG29">
+  <conditionalFormatting sqref="AG10:AG30">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -3387,7 +3484,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG30">
+  <conditionalFormatting sqref="AG31">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3397,7 +3494,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG31:AG35">
+  <conditionalFormatting sqref="AG32:AG36">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3407,7 +3504,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG36:AG40">
+  <conditionalFormatting sqref="AG37:AG41">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3417,7 +3514,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG41">
+  <conditionalFormatting sqref="AG42">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3427,7 +3524,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG42:AG46">
+  <conditionalFormatting sqref="AG43:AG47">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3437,7 +3534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH10:AH29">
+  <conditionalFormatting sqref="AH10:AH30">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3447,7 +3544,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH30">
+  <conditionalFormatting sqref="AH31">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3457,7 +3554,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH31:AH35">
+  <conditionalFormatting sqref="AH32:AH36">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3467,7 +3564,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH36:AH40">
+  <conditionalFormatting sqref="AH37:AH41">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3477,7 +3574,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH41">
+  <conditionalFormatting sqref="AH42">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3487,7 +3584,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH42:AH46">
+  <conditionalFormatting sqref="AH43:AH47">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3497,7 +3594,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C46">
+  <conditionalFormatting sqref="C11:C47">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -3511,7 +3608,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C46">
+  <conditionalFormatting sqref="C10:C47">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -3525,7 +3622,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:AH46">
+  <conditionalFormatting sqref="D10:AH47">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3578,7 +3675,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C11:C46</xm:sqref>
+          <xm:sqref>C11:C47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A2C7A50C-F572-416B-9495-8A28D149BC35}">
@@ -3589,7 +3686,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C10:C46</xm:sqref>
+          <xm:sqref>C10:C47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BCD65580-FCE2-4CC5-9CCE-B782BE912BFA}">

</xml_diff>